<commit_message>
add item policy support
</commit_message>
<xml_diff>
--- a/models/test_data.xlsx
+++ b/models/test_data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reyra\Desktop\DEV\migrate_IZ_to_IZ\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RaphaëlRey\DEV\migrate_IZ_to_IZ\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078BA894-273A-4406-B34E-297D2FE08402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B3EFD3-14ED-4321-A3B1-1F873162C757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1296" yWindow="1800" windowWidth="17268" windowHeight="9060" xr2:uid="{AD365A3D-3304-46D8-98A5-452209B6D1C5}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9420" activeTab="3" xr2:uid="{AD365A3D-3304-46D8-98A5-452209B6D1C5}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Barcodes" sheetId="2" r:id="rId2"/>
     <sheet name="Locations_mapping" sheetId="3" r:id="rId3"/>
-    <sheet name="data_validation" sheetId="4" r:id="rId4"/>
+    <sheet name="Item_policies" sheetId="5" r:id="rId4"/>
+    <sheet name="data_validation" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>Barcode</t>
   </si>
@@ -188,6 +189,18 @@
   </si>
   <si>
     <t>rro_fili</t>
+  </si>
+  <si>
+    <t>*DEFAULT*</t>
+  </si>
+  <si>
+    <t>Source item policy code</t>
+  </si>
+  <si>
+    <t>Destination item policy code</t>
+  </si>
+  <si>
+    <t>01</t>
   </si>
 </sst>
 </file>
@@ -242,13 +255,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -267,7 +282,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -565,11 +580,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D68E6D0E-F394-4B85-9885-9C587EEAF794}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="21.21875" customWidth="1"/>
   </cols>
@@ -634,7 +649,7 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.77734375" customWidth="1"/>
   </cols>
@@ -677,13 +692,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49CD200A-AAE3-41A8-B7B7-08FF5A82F532}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="4" width="25.77734375" customWidth="1"/>
   </cols>
@@ -703,16 +718,26 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>47</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>48</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>49</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>610940001</v>
       </c>
     </row>
@@ -722,6 +747,42 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206F50D4-37BA-4D0A-9619-E97216BE8408}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="23" style="5" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A0D6C5-D024-428E-995D-36256CF838C1}">
   <dimension ref="A1:B31"/>
   <sheetViews>
@@ -729,7 +790,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Force delete source item data too before updating
</commit_message>
<xml_diff>
--- a/models/test_data.xlsx
+++ b/models/test_data.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RaphaëlRey\DEV\migrate_IZ_to_IZ\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2163C6F4-D8F5-4A03-A0E6-10A1C04C598C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B753617F-EF77-4820-A37D-12B2EA6F69B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AD365A3D-3304-46D8-98A5-452209B6D1C5}"/>
+    <workbookView xWindow="3072" yWindow="3072" windowWidth="17280" windowHeight="9420" xr2:uid="{AD365A3D-3304-46D8-98A5-452209B6D1C5}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Barcodes" sheetId="2" r:id="rId2"/>
     <sheet name="Locations_mapping" sheetId="3" r:id="rId3"/>
     <sheet name="Item_policies" sheetId="5" r:id="rId4"/>
-    <sheet name="data_validation" sheetId="4" r:id="rId5"/>
+    <sheet name="data_validation" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -218,10 +218,10 @@
     <t>Fields like 'provenance', 'temp_location', 'temp_library', 'in_temp_location', 'pattern_type', 'statistics_note_1', 'statistics_note_2', 'statistics_note_3', 'po_line' can cause error because the corresponding value doesn't exist maybe in the destination IZ.</t>
   </si>
   <si>
-    <t>In the source IZ delete 'pattern_type'</t>
-  </si>
-  <si>
-    <t>The field 'pattern_type'  if available prevent sometime barcode update.</t>
+    <t>In the source IZ delete delete the fields of items when containing defined values</t>
+  </si>
+  <si>
+    <t>Fields like 'provenance', 'temp_location', 'temp_library', 'in_temp_location', 'pattern_type', 'statistics_note_1', 'statistics_note_2', 'statistics_note_3', 'po_line' can cause error and prevent sometime barcode update (adding prefix "OLD_").</t>
   </si>
 </sst>
 </file>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D68E6D0E-F394-4B85-9885-9C587EEAF794}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
@@ -658,7 +658,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.8">
+    <row r="8" spans="1:4" ht="64.2" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>59</v>
       </c>
@@ -808,7 +808,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>